<commit_message>
Updated delivery_data.xlsx with latest data
</commit_message>
<xml_diff>
--- a/delivery_data.xlsx
+++ b/delivery_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digvi\Desktop\VLC FRANCHISE PROJECT\delivery_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC414E2-4C8A-4BB2-9C3C-8B9D7C269EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F7FE76-D564-44FA-864A-776346F6AB67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="132" windowWidth="21840" windowHeight="12108" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Username</t>
   </si>
@@ -113,6 +113,15 @@
   </si>
   <si>
     <t>static\image3.jpg</t>
+  </si>
+  <si>
+    <t>pista</t>
+  </si>
+  <si>
+    <t>delihvery</t>
+  </si>
+  <si>
+    <t>15kg</t>
   </si>
 </sst>
 </file>
@@ -504,10 +513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,6 +622,26 @@
         <v>25</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45667</v>
+      </c>
+      <c r="D5">
+        <v>1555</v>
+      </c>
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>